<commit_message>
switched sim file from jupyter to py
</commit_message>
<xml_diff>
--- a/results/simulation_res.xlsx
+++ b/results/simulation_res.xlsx
@@ -22,31 +22,31 @@
     <t>min load time</t>
   </si>
   <si>
-    <t>18:44:00</t>
+    <t>18:06:00</t>
+  </si>
+  <si>
+    <t>18:33:00</t>
   </si>
   <si>
     <t>18:49:00</t>
   </si>
   <si>
-    <t>18:37:00</t>
-  </si>
-  <si>
-    <t>18:21:00</t>
-  </si>
-  <si>
-    <t>18:12:00</t>
-  </si>
-  <si>
-    <t>18:31:00</t>
-  </si>
-  <si>
-    <t>18:36:00</t>
-  </si>
-  <si>
-    <t>18:33:00</t>
-  </si>
-  <si>
-    <t>18:58:00</t>
+    <t>18:51:00</t>
+  </si>
+  <si>
+    <t>18:45:00</t>
+  </si>
+  <si>
+    <t>18:42:00</t>
+  </si>
+  <si>
+    <t>18:32:00</t>
+  </si>
+  <si>
+    <t>18:39:00</t>
+  </si>
+  <si>
+    <t>18:03:00</t>
   </si>
 </sst>
 </file>
@@ -423,7 +423,7 @@
         <v>0</v>
       </c>
       <c r="B2">
-        <v>1.02566</v>
+        <v>1.02484</v>
       </c>
       <c r="C2" t="s">
         <v>2</v>
@@ -434,7 +434,7 @@
         <v>1</v>
       </c>
       <c r="B3">
-        <v>1.02589</v>
+        <v>1.02436</v>
       </c>
       <c r="C3" t="s">
         <v>3</v>
@@ -445,7 +445,7 @@
         <v>2</v>
       </c>
       <c r="B4">
-        <v>1.026</v>
+        <v>1.02272</v>
       </c>
       <c r="C4" t="s">
         <v>4</v>
@@ -456,7 +456,7 @@
         <v>3</v>
       </c>
       <c r="B5">
-        <v>1.02403</v>
+        <v>1.02507</v>
       </c>
       <c r="C5" t="s">
         <v>5</v>
@@ -467,10 +467,10 @@
         <v>4</v>
       </c>
       <c r="B6">
-        <v>1.02529</v>
+        <v>1.02475</v>
       </c>
       <c r="C6" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
     </row>
     <row r="7" spans="1:3">
@@ -478,10 +478,10 @@
         <v>5</v>
       </c>
       <c r="B7">
-        <v>1.02518</v>
+        <v>1.02391</v>
       </c>
       <c r="C7" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="8" spans="1:3">
@@ -489,10 +489,10 @@
         <v>6</v>
       </c>
       <c r="B8">
-        <v>1.02533</v>
+        <v>1.02554</v>
       </c>
       <c r="C8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="9" spans="1:3">
@@ -500,10 +500,10 @@
         <v>7</v>
       </c>
       <c r="B9">
-        <v>1.02415</v>
+        <v>1.02534</v>
       </c>
       <c r="C9" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="10" spans="1:3">
@@ -511,10 +511,10 @@
         <v>8</v>
       </c>
       <c r="B10">
-        <v>1.02672</v>
+        <v>1.02481</v>
       </c>
       <c r="C10" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
     </row>
     <row r="11" spans="1:3">
@@ -522,7 +522,7 @@
         <v>9</v>
       </c>
       <c r="B11">
-        <v>1.02312</v>
+        <v>1.02533</v>
       </c>
       <c r="C11" t="s">
         <v>10</v>

</xml_diff>